<commit_message>
add constant parsing to compiler
</commit_message>
<xml_diff>
--- a/fexcel/compile/testdata/test.xlsx
+++ b/fexcel/compile/testdata/test.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{066A9CD9-5028-47C0-B663-A434F1E37130}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4534C84F-6707-4C4F-A03C-FCFB56C8E7CF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1785" windowWidth="12210" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21195" yWindow="3225" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>two</t>
   </si>
@@ -39,6 +39,15 @@
   </si>
   <si>
     <t>jpos</t>
+  </si>
+  <si>
+    <t>Constants</t>
+  </si>
+  <si>
+    <t>HOME_SPEED</t>
+  </si>
+  <si>
+    <t>HOME_CNT</t>
   </si>
 </sst>
 </file>
@@ -350,23 +359,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{587782DA-6CBE-4F87-BF1A-1D517A0FAC1D}">
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:H201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -376,8 +388,14 @@
       <c r="D2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -387,8 +405,14 @@
       <c r="D3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G3" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -399,7 +423,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -410,7 +434,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -421,7 +445,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -432,7 +456,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -440,7 +464,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -448,7 +472,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -456,7 +480,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -464,7 +488,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -472,7 +496,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -480,7 +504,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -488,7 +512,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -496,7 +520,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>